<commit_message>
updated with strain names
</commit_message>
<xml_diff>
--- a/old_database/crypto/bioSample/bioSample_0769.xlsx
+++ b/old_database/crypto/bioSample/bioSample_0769.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/old_database/crypto/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7F967B-E39A-4045-8049-C7383B4ED468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741B9431-8B22-2B40-8E0A-A9B95E6DB9E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="29">
   <si>
     <t>harvestDate</t>
   </si>
@@ -89,6 +89,24 @@
   </si>
   <si>
     <t>90minuteInduction</t>
+  </si>
+  <si>
+    <t>TDY1373</t>
+  </si>
+  <si>
+    <t>TDY1367</t>
+  </si>
+  <si>
+    <t>KN99alpha</t>
+  </si>
+  <si>
+    <t>TDY1256</t>
+  </si>
+  <si>
+    <t>TDY1208</t>
+  </si>
+  <si>
+    <t>TDY1210</t>
   </si>
 </sst>
 </file>
@@ -492,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -549,6 +567,9 @@
       <c r="D2" t="s">
         <v>22</v>
       </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
@@ -575,6 +596,9 @@
       <c r="D3" t="s">
         <v>22</v>
       </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
       <c r="G3" t="s">
         <v>14</v>
       </c>
@@ -601,6 +625,9 @@
       <c r="D4" t="s">
         <v>22</v>
       </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
@@ -627,6 +654,9 @@
       <c r="D5" t="s">
         <v>22</v>
       </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
       <c r="G5" t="s">
         <v>15</v>
       </c>
@@ -653,6 +683,9 @@
       <c r="D6" t="s">
         <v>22</v>
       </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
@@ -679,6 +712,9 @@
       <c r="D7" t="s">
         <v>22</v>
       </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
       <c r="G7" t="s">
         <v>15</v>
       </c>
@@ -705,6 +741,9 @@
       <c r="D8" t="s">
         <v>22</v>
       </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
       <c r="G8" t="s">
         <v>16</v>
       </c>
@@ -731,6 +770,9 @@
       <c r="D9" t="s">
         <v>22</v>
       </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
       <c r="G9" t="s">
         <v>16</v>
       </c>
@@ -757,6 +799,9 @@
       <c r="D10" t="s">
         <v>22</v>
       </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
       <c r="G10" t="s">
         <v>16</v>
       </c>
@@ -783,6 +828,9 @@
       <c r="D11" t="s">
         <v>22</v>
       </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
       <c r="G11" t="s">
         <v>17</v>
       </c>
@@ -809,6 +857,9 @@
       <c r="D12" t="s">
         <v>22</v>
       </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
       <c r="G12" t="s">
         <v>17</v>
       </c>
@@ -834,6 +885,9 @@
       </c>
       <c r="D13" t="s">
         <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
       </c>
       <c r="G13" t="s">
         <v>17</v>
@@ -861,6 +915,9 @@
       <c r="D14" t="s">
         <v>22</v>
       </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
       <c r="G14" t="s">
         <v>14</v>
       </c>
@@ -887,6 +944,9 @@
       <c r="D15" t="s">
         <v>22</v>
       </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
       <c r="G15" t="s">
         <v>14</v>
       </c>
@@ -913,6 +973,9 @@
       <c r="D16" t="s">
         <v>22</v>
       </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
       <c r="G16" t="s">
         <v>14</v>
       </c>
@@ -939,6 +1002,9 @@
       <c r="D17" t="s">
         <v>22</v>
       </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
       <c r="G17" t="s">
         <v>18</v>
       </c>
@@ -965,6 +1031,9 @@
       <c r="D18" t="s">
         <v>22</v>
       </c>
+      <c r="F18" t="s">
+        <v>27</v>
+      </c>
       <c r="G18" t="s">
         <v>18</v>
       </c>
@@ -991,6 +1060,9 @@
       <c r="D19" t="s">
         <v>22</v>
       </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
       <c r="G19" t="s">
         <v>18</v>
       </c>
@@ -1017,6 +1089,9 @@
       <c r="D20" t="s">
         <v>22</v>
       </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
       <c r="G20" t="s">
         <v>19</v>
       </c>
@@ -1043,6 +1118,9 @@
       <c r="D21" t="s">
         <v>22</v>
       </c>
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
       <c r="G21" t="s">
         <v>19</v>
       </c>
@@ -1068,6 +1146,9 @@
       </c>
       <c r="D22" t="s">
         <v>22</v>
+      </c>
+      <c r="F22" t="s">
+        <v>28</v>
       </c>
       <c r="G22" t="s">
         <v>19</v>

</xml_diff>